<commit_message>
add the report for comparing the Nova\/MIUI\/Q qude application.
</commit_message>
<xml_diff>
--- a/task_tencent/desktop compare.xlsx
+++ b/task_tencent/desktop compare.xlsx
@@ -1,18 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
   </bookViews>
   <sheets>
-    <sheet name="总体测试" sheetId="1" r:id="rId1"/>
-    <sheet name="nova菜单树" sheetId="2" r:id="rId2"/>
-    <sheet name="MIUI桌面菜单树" sheetId="3" r:id="rId3"/>
-    <sheet name="Q立方桌面菜单树" sheetId="4" r:id="rId4"/>
+    <sheet name="nova菜单树" sheetId="2" r:id="rId1"/>
+    <sheet name="MIUI桌面菜单树" sheetId="3" r:id="rId2"/>
+    <sheet name="Q立方桌面菜单树" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
@@ -505,42 +504,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="196">
-  <si>
-    <t>测试环境</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Android model:Gionee GN700W
-Android 版本：4.0.4
-内核版本：3.0.13
-分辨率：800*480
-RAM:512MB
-ROM:4GB
-CPU:联发科 MT6577
-CPU频率：双核1024Mhz </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>nova桌面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Miui桌面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Q立方桌面</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>测试软件</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>基本功能</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="189">
   <si>
     <t>nova菜单树</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -1299,7 +1263,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="11">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1314,21 +1278,6 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="黑体"/>
-      <family val="3"/>
-      <charset val="134"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1501,44 +1450,44 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
@@ -1547,28 +1496,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1865,80 +1805,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
-  <cols>
-    <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="24.25" customWidth="1"/>
-    <col min="4" max="4" width="25.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-    </row>
-    <row r="2" spans="1:4" ht="108" customHeight="1">
-      <c r="A2" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-    </row>
-    <row r="3" spans="1:4" ht="27" customHeight="1">
-      <c r="A3" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A3:D3"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor theme="5" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:D111"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" outlineLevelRow="3"/>
@@ -1951,16 +1824,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15">
-      <c r="A1" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
+      <c r="A1" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
     </row>
     <row r="2" spans="1:4" ht="16.5">
       <c r="A2" s="3" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3"/>
@@ -1969,7 +1842,7 @@
     <row r="3" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A3" s="3"/>
       <c r="B3" s="9" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -1978,7 +1851,7 @@
       <c r="A4" s="3"/>
       <c r="B4" s="9"/>
       <c r="C4" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="D4" s="3"/>
     </row>
@@ -1987,7 +1860,7 @@
       <c r="B5" s="9"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="16.5" outlineLevel="3">
@@ -1995,7 +1868,7 @@
       <c r="B6" s="9"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2003,7 +1876,7 @@
       <c r="B7" s="9"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2011,7 +1884,7 @@
       <c r="B8" s="9"/>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2019,7 +1892,7 @@
       <c r="B9" s="9"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2027,7 +1900,7 @@
       <c r="B10" s="9"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2035,14 +1908,14 @@
       <c r="B11" s="9"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A12" s="3"/>
       <c r="B12" s="9"/>
       <c r="C12" s="3" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -2051,7 +1924,7 @@
       <c r="B13" s="9"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2059,7 +1932,7 @@
       <c r="B14" s="9"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2067,14 +1940,14 @@
       <c r="B15" s="9"/>
       <c r="C15" s="3"/>
       <c r="D15" s="3" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A16" s="3"/>
       <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="D16" s="3"/>
     </row>
@@ -2083,7 +1956,7 @@
       <c r="B17" s="9"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="33" outlineLevel="3">
@@ -2091,14 +1964,14 @@
       <c r="B18" s="9"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A19" s="3"/>
       <c r="B19" s="9"/>
       <c r="C19" s="3" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="D19" s="3"/>
     </row>
@@ -2107,7 +1980,7 @@
       <c r="B20" s="9"/>
       <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2115,7 +1988,7 @@
       <c r="B21" s="9"/>
       <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2123,13 +1996,13 @@
       <c r="B22" s="9"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A23" s="3"/>
       <c r="B23" s="9" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
@@ -2138,7 +2011,7 @@
       <c r="A24" s="3"/>
       <c r="B24" s="9"/>
       <c r="C24" s="3" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="D24" s="3"/>
     </row>
@@ -2147,7 +2020,7 @@
       <c r="B25" s="9"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2155,7 +2028,7 @@
       <c r="B26" s="9"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2163,7 +2036,7 @@
       <c r="B27" s="9"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2171,7 +2044,7 @@
       <c r="B28" s="9"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2179,14 +2052,14 @@
       <c r="B29" s="9"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A30" s="3"/>
       <c r="B30" s="9"/>
       <c r="C30" s="3" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="D30" s="3"/>
     </row>
@@ -2195,7 +2068,7 @@
       <c r="B31" s="9"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2203,7 +2076,7 @@
       <c r="B32" s="9"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2211,14 +2084,14 @@
       <c r="B33" s="9"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A34" s="3"/>
       <c r="B34" s="9"/>
       <c r="C34" s="3" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D34" s="3"/>
     </row>
@@ -2227,7 +2100,7 @@
       <c r="B35" s="9"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="33" outlineLevel="2">
@@ -2235,7 +2108,7 @@
       <c r="B36" s="9"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2243,7 +2116,7 @@
       <c r="B37" s="9"/>
       <c r="C37" s="3"/>
       <c r="D37" s="5" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2251,13 +2124,13 @@
       <c r="B38" s="9"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A39" s="3"/>
       <c r="B39" s="9" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -2266,7 +2139,7 @@
       <c r="A40" s="3"/>
       <c r="B40" s="9"/>
       <c r="C40" s="3" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="D40" s="3"/>
     </row>
@@ -2275,7 +2148,7 @@
       <c r="B41" s="9"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2283,7 +2156,7 @@
       <c r="B42" s="9"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2291,7 +2164,7 @@
       <c r="B43" s="9"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2299,7 +2172,7 @@
       <c r="B44" s="9"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2307,7 +2180,7 @@
       <c r="B45" s="9"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2315,7 +2188,7 @@
       <c r="B46" s="9"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2323,7 +2196,7 @@
       <c r="B47" s="9"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2331,7 +2204,7 @@
       <c r="B48" s="9"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2339,7 +2212,7 @@
       <c r="B49" s="9"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2347,14 +2220,14 @@
       <c r="B50" s="9"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A51" s="3"/>
       <c r="B51" s="9"/>
       <c r="C51" s="3" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="D51" s="3"/>
     </row>
@@ -2363,7 +2236,7 @@
       <c r="B52" s="9"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2371,13 +2244,13 @@
       <c r="B53" s="9"/>
       <c r="C53" s="3"/>
       <c r="D53" s="5" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A54" s="3"/>
       <c r="B54" s="9" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C54" s="3"/>
       <c r="D54" s="3"/>
@@ -2386,7 +2259,7 @@
       <c r="A55" s="3"/>
       <c r="B55" s="9"/>
       <c r="C55" s="3" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="D55" s="3"/>
     </row>
@@ -2395,7 +2268,7 @@
       <c r="B56" s="9"/>
       <c r="C56" s="3"/>
       <c r="D56" s="3" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2403,14 +2276,14 @@
       <c r="B57" s="9"/>
       <c r="C57" s="3"/>
       <c r="D57" s="3" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A58" s="3"/>
       <c r="B58" s="9"/>
       <c r="C58" s="3" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="D58" s="3"/>
     </row>
@@ -2419,7 +2292,7 @@
       <c r="B59" s="9"/>
       <c r="C59" s="3"/>
       <c r="D59" s="3" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2427,13 +2300,13 @@
       <c r="B60" s="9"/>
       <c r="C60" s="3"/>
       <c r="D60" s="3" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A61" s="3"/>
       <c r="B61" s="9" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
@@ -2442,7 +2315,7 @@
       <c r="A62" s="3"/>
       <c r="B62" s="9"/>
       <c r="C62" s="3" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="D62" s="3"/>
     </row>
@@ -2451,7 +2324,7 @@
       <c r="B63" s="9"/>
       <c r="C63" s="3"/>
       <c r="D63" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2459,7 +2332,7 @@
       <c r="B64" s="9"/>
       <c r="C64" s="3"/>
       <c r="D64" s="3" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2467,7 +2340,7 @@
       <c r="B65" s="9"/>
       <c r="C65" s="3"/>
       <c r="D65" s="3" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2475,7 +2348,7 @@
       <c r="B66" s="9"/>
       <c r="C66" s="3"/>
       <c r="D66" s="3" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2483,7 +2356,7 @@
       <c r="B67" s="9"/>
       <c r="C67" s="3"/>
       <c r="D67" s="3" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2491,7 +2364,7 @@
       <c r="B68" s="9"/>
       <c r="C68" s="3"/>
       <c r="D68" s="3" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2499,14 +2372,14 @@
       <c r="B69" s="9"/>
       <c r="C69" s="3"/>
       <c r="D69" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A70" s="3"/>
       <c r="B70" s="9"/>
       <c r="C70" s="3" t="s">
-        <v>81</v>
+        <v>74</v>
       </c>
       <c r="D70" s="3"/>
     </row>
@@ -2515,7 +2388,7 @@
       <c r="B71" s="9"/>
       <c r="C71" s="3"/>
       <c r="D71" s="3" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2523,13 +2396,13 @@
       <c r="B72" s="9"/>
       <c r="C72" s="3"/>
       <c r="D72" s="3" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A73" s="3"/>
       <c r="B73" s="9" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="C73" s="3"/>
       <c r="D73" s="3"/>
@@ -2538,7 +2411,7 @@
       <c r="A74" s="3"/>
       <c r="B74" s="9"/>
       <c r="C74" s="3" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="D74" s="3"/>
     </row>
@@ -2547,7 +2420,7 @@
       <c r="B75" s="9"/>
       <c r="C75" s="3"/>
       <c r="D75" s="3" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2555,7 +2428,7 @@
       <c r="B76" s="9"/>
       <c r="C76" s="3"/>
       <c r="D76" s="3" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="16.5" outlineLevel="3">
@@ -2563,14 +2436,14 @@
       <c r="B77" s="9"/>
       <c r="C77" s="3"/>
       <c r="D77" s="3" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="16.5" outlineLevel="2">
       <c r="A78" s="3"/>
       <c r="B78" s="9"/>
       <c r="C78" s="3" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="D78" s="3"/>
     </row>
@@ -2579,7 +2452,7 @@
       <c r="B79" s="9"/>
       <c r="C79" s="3"/>
       <c r="D79" s="6" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2587,7 +2460,7 @@
       <c r="B80" s="9"/>
       <c r="C80" s="3"/>
       <c r="D80" s="6" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2595,7 +2468,7 @@
       <c r="B81" s="9"/>
       <c r="C81" s="3"/>
       <c r="D81" s="6" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2603,7 +2476,7 @@
       <c r="B82" s="9"/>
       <c r="C82" s="3"/>
       <c r="D82" s="6" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2611,7 +2484,7 @@
       <c r="B83" s="9"/>
       <c r="C83" s="3"/>
       <c r="D83" s="6" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2619,7 +2492,7 @@
       <c r="B84" s="9"/>
       <c r="C84" s="3"/>
       <c r="D84" s="6" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="16.5" outlineLevel="2">
@@ -2627,7 +2500,7 @@
       <c r="B85" s="9"/>
       <c r="C85" s="3"/>
       <c r="D85" s="6" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="33" outlineLevel="2">
@@ -2635,7 +2508,7 @@
       <c r="B86" s="9"/>
       <c r="C86" s="3"/>
       <c r="D86" s="6" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="33" outlineLevel="2">
@@ -2643,13 +2516,13 @@
       <c r="B87" s="9"/>
       <c r="C87" s="3"/>
       <c r="D87" s="6" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A88" s="3"/>
       <c r="B88" s="9" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C88" s="3"/>
       <c r="D88" s="3"/>
@@ -2657,7 +2530,7 @@
     <row r="89" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A89" s="3"/>
       <c r="B89" s="9" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C89" s="3"/>
       <c r="D89" s="3"/>
@@ -2666,7 +2539,7 @@
       <c r="A90" s="3"/>
       <c r="B90" s="9"/>
       <c r="C90" s="3" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="D90" s="3"/>
     </row>
@@ -2674,7 +2547,7 @@
       <c r="A91" s="3"/>
       <c r="B91" s="9"/>
       <c r="C91" s="3" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="D91" s="3"/>
     </row>
@@ -2682,14 +2555,14 @@
       <c r="A92" s="3"/>
       <c r="B92" s="9"/>
       <c r="C92" s="3" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D92" s="3"/>
     </row>
     <row r="93" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A93" s="3"/>
       <c r="B93" s="9" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="C93" s="3"/>
       <c r="D93" s="3"/>
@@ -2698,7 +2571,7 @@
       <c r="A94" s="3"/>
       <c r="B94" s="9"/>
       <c r="C94" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="D94" s="3"/>
     </row>
@@ -2706,7 +2579,7 @@
       <c r="A95" s="3"/>
       <c r="B95" s="9"/>
       <c r="C95" s="3" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D95" s="3"/>
     </row>
@@ -2714,7 +2587,7 @@
       <c r="A96" s="3"/>
       <c r="B96" s="9"/>
       <c r="C96" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="D96" s="3"/>
     </row>
@@ -2722,13 +2595,13 @@
       <c r="A97" s="3"/>
       <c r="B97" s="9"/>
       <c r="C97" s="3" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="D97" s="3"/>
     </row>
     <row r="98" spans="1:4" ht="16.5">
       <c r="A98" s="3" t="s">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="B98" s="9"/>
       <c r="C98" s="3"/>
@@ -2737,7 +2610,7 @@
     <row r="99" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A99" s="3"/>
       <c r="B99" s="7" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="C99" s="3"/>
       <c r="D99" s="3"/>
@@ -2745,7 +2618,7 @@
     <row r="100" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A100" s="3"/>
       <c r="B100" s="7" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C100" s="3"/>
       <c r="D100" s="3"/>
@@ -2753,7 +2626,7 @@
     <row r="101" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A101" s="3"/>
       <c r="B101" s="7" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C101" s="3"/>
       <c r="D101" s="3"/>
@@ -2761,14 +2634,14 @@
     <row r="102" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A102" s="3"/>
       <c r="B102" s="8" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C102" s="3"/>
       <c r="D102" s="3"/>
     </row>
     <row r="103" spans="1:4" ht="16.5">
       <c r="A103" s="3" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -2777,7 +2650,7 @@
     <row r="104" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A104" s="3"/>
       <c r="B104" s="3" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C104" s="3"/>
       <c r="D104" s="3"/>
@@ -2785,7 +2658,7 @@
     <row r="105" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A105" s="3"/>
       <c r="B105" s="3" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C105" s="3"/>
       <c r="D105" s="3"/>
@@ -2793,14 +2666,14 @@
     <row r="106" spans="1:4" ht="16.5" outlineLevel="1">
       <c r="A106" s="3"/>
       <c r="B106" s="3" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
     </row>
     <row r="107" spans="1:4" ht="19.5" customHeight="1">
       <c r="A107" s="3" t="s">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -2829,7 +2702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E40"/>
   <sheetViews>
@@ -2847,17 +2720,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5">
-      <c r="A1" s="19" t="s">
-        <v>114</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
+      <c r="A1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
     </row>
     <row r="2" spans="1:5" ht="16.5">
       <c r="A2" s="11" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2866,7 +2739,7 @@
     </row>
     <row r="3" spans="1:5" ht="16.5">
       <c r="A3" s="11" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -2875,7 +2748,7 @@
     </row>
     <row r="4" spans="1:5" ht="16.5">
       <c r="A4" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -2884,7 +2757,7 @@
     </row>
     <row r="5" spans="1:5" ht="16.5">
       <c r="A5" s="11" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
@@ -2893,7 +2766,7 @@
     </row>
     <row r="6" spans="1:5" ht="16.5">
       <c r="A6" s="11" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -2902,7 +2775,7 @@
     </row>
     <row r="7" spans="1:5" ht="16.5">
       <c r="A7" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -2912,7 +2785,7 @@
     <row r="8" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A8" s="2"/>
       <c r="B8" s="12" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -2922,7 +2795,7 @@
       <c r="A9" s="2"/>
       <c r="B9" s="12"/>
       <c r="C9" s="2" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -2932,7 +2805,7 @@
       <c r="B10" s="12"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="E10" s="2"/>
     </row>
@@ -2941,7 +2814,7 @@
       <c r="B11" s="12"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="E11" s="2"/>
     </row>
@@ -2951,7 +2824,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="16.5" outlineLevel="4">
@@ -2960,7 +2833,7 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="16.5" outlineLevel="4">
@@ -2969,7 +2842,7 @@
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="16.5" outlineLevel="4">
@@ -2978,7 +2851,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="16.5" outlineLevel="4">
@@ -2987,7 +2860,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="16.5" outlineLevel="4">
@@ -2996,7 +2869,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:5" ht="16.5" outlineLevel="3">
@@ -3004,7 +2877,7 @@
       <c r="B18" s="12"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -3014,7 +2887,7 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="16.5" outlineLevel="3">
@@ -3023,14 +2896,14 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16.5" outlineLevel="2">
       <c r="A21" s="2"/>
       <c r="B21" s="12"/>
       <c r="C21" s="2" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -3040,7 +2913,7 @@
       <c r="B22" s="12"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -3049,7 +2922,7 @@
       <c r="B23" s="12"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E23" s="2"/>
     </row>
@@ -3058,7 +2931,7 @@
       <c r="B24" s="12"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E24" s="2"/>
     </row>
@@ -3067,7 +2940,7 @@
       <c r="B25" s="12"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -3076,7 +2949,7 @@
       <c r="B26" s="12"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E26" s="2"/>
     </row>
@@ -3085,7 +2958,7 @@
       <c r="B27" s="12"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E27" s="2"/>
     </row>
@@ -3093,7 +2966,7 @@
       <c r="A28" s="2"/>
       <c r="B28" s="12"/>
       <c r="C28" s="2" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -3103,7 +2976,7 @@
       <c r="B29" s="12"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="E29" s="2"/>
     </row>
@@ -3112,7 +2985,7 @@
       <c r="B30" s="12"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E30" s="2"/>
     </row>
@@ -3121,14 +2994,14 @@
       <c r="B31" s="12"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A32" s="2"/>
       <c r="B32" s="12" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -3138,7 +3011,7 @@
       <c r="A33" s="2"/>
       <c r="B33" s="12"/>
       <c r="C33" s="2" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -3148,7 +3021,7 @@
       <c r="B34" s="12"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E34" s="2"/>
     </row>
@@ -3157,7 +3030,7 @@
       <c r="B35" s="12"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="E35" s="2"/>
     </row>
@@ -3165,7 +3038,7 @@
       <c r="A36" s="2"/>
       <c r="B36" s="12"/>
       <c r="C36" s="2" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -3173,7 +3046,7 @@
     <row r="37" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A37" s="2"/>
       <c r="B37" s="12" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
@@ -3183,7 +3056,7 @@
       <c r="A38" s="2"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
@@ -3192,7 +3065,7 @@
       <c r="A39" s="2"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
@@ -3201,7 +3074,7 @@
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -3217,11 +3090,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
@@ -3235,17 +3108,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="16.5">
-      <c r="A1" s="20" t="s">
-        <v>195</v>
-      </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22"/>
+      <c r="A1" s="17" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="19"/>
     </row>
     <row r="2" spans="1:5" ht="16.5">
       <c r="A2" s="2" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -3255,7 +3128,7 @@
     <row r="3" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
@@ -3264,7 +3137,7 @@
     <row r="4" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A4" s="2"/>
       <c r="B4" s="2" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3273,7 +3146,7 @@
     <row r="5" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A5" s="2"/>
       <c r="B5" s="2" t="s">
-        <v>164</v>
+        <v>157</v>
       </c>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -3281,7 +3154,7 @@
     </row>
     <row r="6" spans="1:5" ht="16.5">
       <c r="A6" s="2" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
@@ -3290,7 +3163,7 @@
     </row>
     <row r="7" spans="1:5" ht="16.5">
       <c r="A7" s="2" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
@@ -3299,7 +3172,7 @@
     </row>
     <row r="8" spans="1:5" ht="16.5">
       <c r="A8" s="2" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -3309,7 +3182,7 @@
     <row r="9" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A9" s="2"/>
       <c r="B9" s="2" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -3318,7 +3191,7 @@
     <row r="10" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A10" s="2"/>
       <c r="B10" s="2" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -3326,7 +3199,7 @@
     </row>
     <row r="11" spans="1:5" ht="16.5">
       <c r="A11" s="2" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
@@ -3335,7 +3208,7 @@
     </row>
     <row r="12" spans="1:5" ht="16.5">
       <c r="A12" s="2" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -3344,7 +3217,7 @@
     </row>
     <row r="13" spans="1:5" ht="16.5">
       <c r="A13" s="2" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
@@ -3354,7 +3227,7 @@
     <row r="14" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A14" s="2"/>
       <c r="B14" s="2" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -3363,7 +3236,7 @@
     <row r="15" spans="1:5" ht="16.5" outlineLevel="1">
       <c r="A15" s="2"/>
       <c r="B15" s="2" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -3373,7 +3246,7 @@
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -3382,7 +3255,7 @@
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
@@ -3391,7 +3264,7 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -3401,7 +3274,7 @@
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E19" s="2"/>
     </row>
@@ -3411,7 +3284,7 @@
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
-        <v>183</v>
+        <v>176</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="16.5" hidden="1" outlineLevel="4">
@@ -3420,7 +3293,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>184</v>
+        <v>177</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="16.5" hidden="1" outlineLevel="3">
@@ -3428,7 +3301,7 @@
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="E22" s="2"/>
     </row>
@@ -3438,7 +3311,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="16.5" hidden="1" outlineLevel="4">
@@ -3447,7 +3320,7 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="16.5" hidden="1" outlineLevel="3">
@@ -3455,7 +3328,7 @@
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>182</v>
+        <v>175</v>
       </c>
       <c r="E25" s="2"/>
     </row>
@@ -3465,7 +3338,7 @@
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2" t="s">
-        <v>187</v>
+        <v>180</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="16.5" hidden="1" outlineLevel="3">
@@ -3474,14 +3347,14 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2" t="s">
-        <v>188</v>
+        <v>181</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="16.5" hidden="1" outlineLevel="2">
       <c r="A28" s="2"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -3489,7 +3362,7 @@
     <row r="29" spans="1:5" ht="16.5" outlineLevel="1" collapsed="1">
       <c r="A29" s="2"/>
       <c r="B29" s="2" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -3499,7 +3372,7 @@
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -3509,7 +3382,7 @@
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="E31" s="2"/>
     </row>
@@ -3518,7 +3391,7 @@
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2" t="s">
-        <v>190</v>
+        <v>183</v>
       </c>
       <c r="E32" s="2"/>
     </row>
@@ -3528,7 +3401,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2" t="s">
-        <v>191</v>
+        <v>184</v>
       </c>
     </row>
     <row r="34" spans="1:5" ht="16.5" hidden="1" outlineLevel="3">
@@ -3537,14 +3410,14 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2" t="s">
-        <v>192</v>
+        <v>185</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="16.5" hidden="1" outlineLevel="2">
       <c r="A35" s="2"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -3552,7 +3425,7 @@
     <row r="36" spans="1:5" ht="16.5" outlineLevel="1" collapsed="1">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
@@ -3562,7 +3435,7 @@
       <c r="A37" s="2"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -3572,7 +3445,7 @@
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="E38" s="2"/>
     </row>
@@ -3581,7 +3454,7 @@
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="E39" s="2"/>
     </row>
@@ -3589,7 +3462,7 @@
       <c r="A40" s="2"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
@@ -3598,14 +3471,14 @@
       <c r="A41" s="2"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:5" ht="16.5">
       <c r="A42" s="2" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>

</xml_diff>